<commit_message>
update retirando pasta metada e recommenders
</commit_message>
<xml_diff>
--- a/ReservarUmTicket/data/SampleAppDataMassa.xlsx
+++ b/ReservarUmTicket/data/SampleAppDataMassa.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPERFOMACE\ReservarUmTicket\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0136412A-234A-453C-AFDD-D5864756890A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B4B130-19A9-4FE8-B5EF-8A8EC5D0B0DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>FlightNumber</t>
   </si>
@@ -94,6 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -490,19 +491,19 @@
   <dimension ref="A1:IS9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.25" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="253" width="9.125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="21.25" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="23.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="18.875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="18.125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="18.125" collapsed="true"/>
+    <col min="8" max="253" customWidth="true" style="1" width="9.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75">
@@ -547,7 +548,9 @@
       <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11"/>
+      <c r="G2" s="11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15">
       <c r="A3" s="7" t="s">
@@ -569,6 +572,9 @@
         <v>6</v>
       </c>
       <c r="G3" s="6"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:7">
       <c r="E9" s="10"/>

</xml_diff>